<commit_message>
Removing extraneous quotation marks
</commit_message>
<xml_diff>
--- a/examples/1_1_Metabolomics_Draft/MTBLS263.xlsx
+++ b/examples/1_1_Metabolomics_Draft/MTBLS263.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19485" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="MTBLS263" sheetId="1" r:id="rId1"/>
@@ -1550,7 +1550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2259,31 +2261,31 @@
         <v>56.442399999999999</v>
       </c>
       <c r="Q55">
-        <v>59809754.6237</v>
+        <v>59809754.619999997</v>
       </c>
       <c r="R55">
-        <v>63773291.215999998</v>
+        <v>63773291.219999999</v>
       </c>
       <c r="S55">
-        <v>61630638.374300003</v>
+        <v>61630638.369999997</v>
       </c>
       <c r="T55">
-        <v>59131129.426600002</v>
+        <v>59131129.43</v>
       </c>
       <c r="U55">
-        <v>63874747.953900002</v>
+        <v>63874747.950000003</v>
       </c>
       <c r="V55">
-        <v>66320708.839900002</v>
+        <v>66320708.840000004</v>
       </c>
       <c r="W55">
-        <v>185213684.21399999</v>
+        <v>185213684.19999999</v>
       </c>
       <c r="X55">
         <v>3.2134999999999998</v>
       </c>
       <c r="Y55">
-        <v>189326586.22029999</v>
+        <v>189326586.19999999</v>
       </c>
       <c r="Z55">
         <v>5.7923</v>
@@ -2342,31 +2344,31 @@
         <v>44.024900000000002</v>
       </c>
       <c r="Q56">
-        <v>1164487.3163999999</v>
+        <v>1164487.3160000001</v>
       </c>
       <c r="R56">
-        <v>1376477.9739000001</v>
+        <v>1376477.9739999999</v>
       </c>
       <c r="S56">
-        <v>1531498.6980999999</v>
+        <v>1531498.6980000001</v>
       </c>
       <c r="T56">
         <v>1398304.361</v>
       </c>
       <c r="U56">
-        <v>1633581.6309</v>
+        <v>1633581.6310000001</v>
       </c>
       <c r="V56">
-        <v>2129396.5118</v>
+        <v>2129396.5120000001</v>
       </c>
       <c r="W56">
-        <v>4072463.9884000001</v>
+        <v>4072463.9879999999</v>
       </c>
       <c r="X56">
         <v>13.5722</v>
       </c>
       <c r="Y56">
-        <v>5161282.5036000004</v>
+        <v>5161282.5039999997</v>
       </c>
       <c r="Z56">
         <v>21.692499999999999</v>
@@ -2425,31 +2427,31 @@
         <v>48.2759</v>
       </c>
       <c r="Q57">
-        <v>65543883.463200003</v>
+        <v>65543883.460000001</v>
       </c>
       <c r="R57">
-        <v>65475290.353500001</v>
+        <v>65475290.350000001</v>
       </c>
       <c r="S57">
-        <v>67694647.592700005</v>
+        <v>67694647.590000004</v>
       </c>
       <c r="T57">
-        <v>59237651.351800002</v>
+        <v>59237651.350000001</v>
       </c>
       <c r="U57">
-        <v>56077561.474399999</v>
+        <v>56077561.469999999</v>
       </c>
       <c r="V57">
         <v>54207405.409999996</v>
       </c>
       <c r="W57">
-        <v>198713821.40939999</v>
+        <v>198713821.40000001</v>
       </c>
       <c r="X57">
         <v>1.9053</v>
       </c>
       <c r="Y57">
-        <v>169522618.2362</v>
+        <v>169522618.19999999</v>
       </c>
       <c r="Z57">
         <v>4.4995000000000003</v>
@@ -2511,28 +2513,28 @@
         <v>8419806.0460000001</v>
       </c>
       <c r="R58">
-        <v>7954686.9192000004</v>
+        <v>7954686.9189999998</v>
       </c>
       <c r="S58">
-        <v>8318226.5612000003</v>
+        <v>8318226.5609999998</v>
       </c>
       <c r="T58">
-        <v>8007517.5916999998</v>
+        <v>8007517.5920000002</v>
       </c>
       <c r="U58">
-        <v>7319791.0674000001</v>
+        <v>7319791.0669999998</v>
       </c>
       <c r="V58">
-        <v>7367477.8015999999</v>
+        <v>7367477.8020000001</v>
       </c>
       <c r="W58">
-        <v>24692719.5264</v>
+        <v>24692719.530000001</v>
       </c>
       <c r="X58">
         <v>2.9710999999999999</v>
       </c>
       <c r="Y58">
-        <v>22694786.460700002</v>
+        <v>22694786.460000001</v>
       </c>
       <c r="Z58">
         <v>5.0765000000000002</v>
@@ -2591,31 +2593,31 @@
         <v>48.710500000000003</v>
       </c>
       <c r="Q59">
-        <v>21775405.563700002</v>
+        <v>21775405.559999999</v>
       </c>
       <c r="R59">
-        <v>23532222.5744</v>
+        <v>23532222.57</v>
       </c>
       <c r="S59">
-        <v>24850183.034699999</v>
+        <v>24850183.030000001</v>
       </c>
       <c r="T59">
-        <v>18841152.121199999</v>
+        <v>18841152.120000001</v>
       </c>
       <c r="U59">
-        <v>22892660.203000002</v>
+        <v>22892660.199999999</v>
       </c>
       <c r="V59">
-        <v>21760739.432300001</v>
+        <v>21760739.43</v>
       </c>
       <c r="W59">
-        <v>70157811.172800004</v>
+        <v>70157811.170000002</v>
       </c>
       <c r="X59">
         <v>6.5963000000000003</v>
       </c>
       <c r="Y59">
-        <v>63494551.756499998</v>
+        <v>63494551.759999998</v>
       </c>
       <c r="Z59">
         <v>9.8770000000000007</v>
@@ -2674,31 +2676,31 @@
         <v>45.886800000000001</v>
       </c>
       <c r="Q60">
-        <v>59134552.300300002</v>
+        <v>59134552.299999997</v>
       </c>
       <c r="R60">
-        <v>57461952.471000001</v>
+        <v>57461952.469999999</v>
       </c>
       <c r="S60">
-        <v>60069535.598499998</v>
+        <v>60069535.600000001</v>
       </c>
       <c r="T60">
-        <v>55657781.216499999</v>
+        <v>55657781.219999999</v>
       </c>
       <c r="U60">
-        <v>56998852.392999999</v>
+        <v>56998852.390000001</v>
       </c>
       <c r="V60">
-        <v>60837200.274300002</v>
+        <v>60837200.270000003</v>
       </c>
       <c r="W60">
-        <v>176666040.3698</v>
+        <v>176666040.40000001</v>
       </c>
       <c r="X60">
         <v>2.2433000000000001</v>
       </c>
       <c r="Y60">
-        <v>173493833.8838</v>
+        <v>173493833.90000001</v>
       </c>
       <c r="Z60">
         <v>4.6482999999999999</v>
@@ -2757,31 +2759,31 @@
         <v>44.523800000000001</v>
       </c>
       <c r="Q61">
-        <v>6594546.7669000002</v>
+        <v>6594546.767</v>
       </c>
       <c r="R61">
-        <v>6679574.3863000004</v>
+        <v>6679574.3859999999</v>
       </c>
       <c r="S61">
-        <v>6147241.6140999999</v>
+        <v>6147241.6140000001</v>
       </c>
       <c r="T61">
         <v>6238970.0020000003</v>
       </c>
       <c r="U61">
-        <v>6287508.4829000002</v>
+        <v>6287508.483</v>
       </c>
       <c r="V61">
-        <v>7032912.1431999998</v>
+        <v>7032912.1430000002</v>
       </c>
       <c r="W61">
-        <v>19421362.7674</v>
+        <v>19421362.77</v>
       </c>
       <c r="X61">
         <v>4.4173999999999998</v>
       </c>
       <c r="Y61">
-        <v>19559390.6281</v>
+        <v>19559390.629999999</v>
       </c>
       <c r="Z61">
         <v>6.8258999999999999</v>
@@ -2840,31 +2842,31 @@
         <v>49.309199999999997</v>
       </c>
       <c r="Q62">
-        <v>8652081.2982999999</v>
+        <v>8652081.2980000004</v>
       </c>
       <c r="R62">
-        <v>8068845.0382000003</v>
+        <v>8068845.0379999997</v>
       </c>
       <c r="S62">
-        <v>8480535.2914000005</v>
+        <v>8480535.2909999993</v>
       </c>
       <c r="T62">
-        <v>7567115.7922999999</v>
+        <v>7567115.7920000004</v>
       </c>
       <c r="U62">
-        <v>9299021.4272000007</v>
+        <v>9299021.4269999992</v>
       </c>
       <c r="V62">
-        <v>8807513.5660999995</v>
+        <v>8807513.5659999996</v>
       </c>
       <c r="W62">
-        <v>25201461.627900001</v>
+        <v>25201461.629999999</v>
       </c>
       <c r="X62">
         <v>3.5682</v>
       </c>
       <c r="Y62">
-        <v>25673650.785500001</v>
+        <v>25673650.789999999</v>
       </c>
       <c r="Z62">
         <v>10.4293</v>
@@ -2923,31 +2925,31 @@
         <v>52.851500000000001</v>
       </c>
       <c r="Q63">
-        <v>5928286.9356000004</v>
+        <v>5928286.9359999998</v>
       </c>
       <c r="R63">
-        <v>5417515.3289000001</v>
+        <v>5417515.3289999999</v>
       </c>
       <c r="S63">
-        <v>5820192.7697000001</v>
+        <v>5820192.7699999996</v>
       </c>
       <c r="T63">
-        <v>6318313.4423000002</v>
+        <v>6318313.4419999998</v>
       </c>
       <c r="U63">
-        <v>7358851.5428999998</v>
+        <v>7358851.5429999996</v>
       </c>
       <c r="V63">
-        <v>6698599.7855000002</v>
+        <v>6698599.7860000003</v>
       </c>
       <c r="W63">
-        <v>17165995.034200002</v>
+        <v>17165995.030000001</v>
       </c>
       <c r="X63">
         <v>4.7042000000000002</v>
       </c>
       <c r="Y63">
-        <v>20375764.770599999</v>
+        <v>20375764.77</v>
       </c>
       <c r="Z63">
         <v>7.7519999999999998</v>
@@ -3006,31 +3008,31 @@
         <v>47.621200000000002</v>
       </c>
       <c r="Q64">
-        <v>8552283.8278999999</v>
+        <v>8552283.8279999997</v>
       </c>
       <c r="R64">
-        <v>7430405.0947000002</v>
+        <v>7430405.0949999997</v>
       </c>
       <c r="S64">
-        <v>8442646.2336999997</v>
+        <v>8442646.2339999992</v>
       </c>
       <c r="T64">
-        <v>10530094.7552</v>
+        <v>10530094.76</v>
       </c>
       <c r="U64">
-        <v>10328394.761499999</v>
+        <v>10328394.76</v>
       </c>
       <c r="V64">
-        <v>12041933.178200001</v>
+        <v>12041933.18</v>
       </c>
       <c r="W64">
-        <v>24425335.156199999</v>
+        <v>24425335.16</v>
       </c>
       <c r="X64">
         <v>7.5965999999999996</v>
       </c>
       <c r="Y64">
-        <v>32900422.694899999</v>
+        <v>32900422.690000001</v>
       </c>
       <c r="Z64">
         <v>8.5396999999999998</v>
@@ -3092,28 +3094,28 @@
         <v>2465240.29</v>
       </c>
       <c r="R65">
-        <v>2312034.2787000001</v>
+        <v>2312034.2790000001</v>
       </c>
       <c r="S65">
-        <v>2478860.3385000001</v>
+        <v>2478860.3390000002</v>
       </c>
       <c r="T65">
-        <v>1261327.8343</v>
+        <v>1261327.834</v>
       </c>
       <c r="U65">
-        <v>1504831.4823</v>
+        <v>1504831.4820000001</v>
       </c>
       <c r="V65">
-        <v>1670066.4952</v>
+        <v>1670066.4950000001</v>
       </c>
       <c r="W65">
-        <v>7256134.9072000002</v>
+        <v>7256134.9069999997</v>
       </c>
       <c r="X65">
         <v>3.83</v>
       </c>
       <c r="Y65">
-        <v>4436225.8118000003</v>
+        <v>4436225.8119999999</v>
       </c>
       <c r="Z65">
         <v>13.9047</v>
@@ -3172,31 +3174,31 @@
         <v>47.440100000000001</v>
       </c>
       <c r="Q66">
-        <v>27880437.270300001</v>
+        <v>27880437.27</v>
       </c>
       <c r="R66">
-        <v>28389759.044</v>
+        <v>28389759.039999999</v>
       </c>
       <c r="S66">
-        <v>27913260.295400001</v>
+        <v>27913260.300000001</v>
       </c>
       <c r="T66">
-        <v>39816663.528999999</v>
+        <v>39816663.530000001</v>
       </c>
       <c r="U66">
-        <v>44101276.592500001</v>
+        <v>44101276.590000004</v>
       </c>
       <c r="V66">
-        <v>43411662.291199997</v>
+        <v>43411662.289999999</v>
       </c>
       <c r="W66">
-        <v>84183456.609699994</v>
+        <v>84183456.609999999</v>
       </c>
       <c r="X66">
         <v>1.0158</v>
       </c>
       <c r="Y66">
-        <v>127329602.4128</v>
+        <v>127329602.40000001</v>
       </c>
       <c r="Z66">
         <v>5.4204999999999997</v>
@@ -3338,13 +3340,13 @@
         <v>53.395699999999998</v>
       </c>
       <c r="Q68">
-        <v>1321073.9612</v>
+        <v>1321073.9609999999</v>
       </c>
       <c r="R68">
-        <v>1417953.1494</v>
+        <v>1417953.149</v>
       </c>
       <c r="S68">
-        <v>1424344.2490999999</v>
+        <v>1424344.2490000001</v>
       </c>
       <c r="T68">
         <v>0</v>
@@ -3356,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="W68">
-        <v>4163371.3596000001</v>
+        <v>4163371.36</v>
       </c>
       <c r="X68">
         <v>4.1696999999999997</v>
@@ -3522,13 +3524,13 @@
         <v>682375.61490000004</v>
       </c>
       <c r="W70">
-        <v>2413050.4583000001</v>
+        <v>2413050.4580000001</v>
       </c>
       <c r="X70">
         <v>3.1331000000000002</v>
       </c>
       <c r="Y70">
-        <v>1964459.8718000001</v>
+        <v>1964459.872</v>
       </c>
       <c r="Z70">
         <v>13.615500000000001</v>
@@ -3587,31 +3589,31 @@
         <v>53.892499999999998</v>
       </c>
       <c r="Q71">
-        <v>19440344.687199999</v>
+        <v>19440344.690000001</v>
       </c>
       <c r="R71">
-        <v>19514108.6274</v>
+        <v>19514108.629999999</v>
       </c>
       <c r="S71">
-        <v>17696364.207400002</v>
+        <v>17696364.210000001</v>
       </c>
       <c r="T71">
         <v>11477221.32</v>
       </c>
       <c r="U71">
-        <v>13726671.6094</v>
+        <v>13726671.609999999</v>
       </c>
       <c r="V71">
-        <v>15013706.8378</v>
+        <v>15013706.84</v>
       </c>
       <c r="W71">
-        <v>56650817.522</v>
+        <v>56650817.520000003</v>
       </c>
       <c r="X71">
         <v>5.4482999999999997</v>
       </c>
       <c r="Y71">
-        <v>40217599.767200001</v>
+        <v>40217599.770000003</v>
       </c>
       <c r="Z71">
         <v>13.351900000000001</v>
@@ -3708,22 +3710,22 @@
         <v>447.87</v>
       </c>
       <c r="L74">
-        <v>59579140.667599998</v>
+        <v>59579140.670000002</v>
       </c>
       <c r="M74">
-        <v>63545698.187899999</v>
+        <v>63545698.189999998</v>
       </c>
       <c r="N74">
-        <v>61393680.886</v>
+        <v>61393680.890000001</v>
       </c>
       <c r="O74">
-        <v>59131129.426600002</v>
+        <v>59131129.43</v>
       </c>
       <c r="P74">
-        <v>63693769.300800003</v>
+        <v>63693769.299999997</v>
       </c>
       <c r="Q74">
-        <v>66308065.774999999</v>
+        <v>66308065.780000001</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
@@ -3761,22 +3763,22 @@
         <v>648.11</v>
       </c>
       <c r="L75">
-        <v>59134552.300300002</v>
+        <v>59134552.299999997</v>
       </c>
       <c r="M75">
-        <v>57461952.471000001</v>
+        <v>57461952.469999999</v>
       </c>
       <c r="N75">
-        <v>60069535.598499998</v>
+        <v>60069535.600000001</v>
       </c>
       <c r="O75">
-        <v>55657781.216499999</v>
+        <v>55657781.219999999</v>
       </c>
       <c r="P75">
-        <v>56998852.392999999</v>
+        <v>56998852.390000001</v>
       </c>
       <c r="Q75">
-        <v>60837200.274300002</v>
+        <v>60837200.270000003</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
@@ -3814,19 +3816,19 @@
         <v>541.07000000000005</v>
       </c>
       <c r="L76">
-        <v>65543883.463200003</v>
+        <v>65543883.460000001</v>
       </c>
       <c r="M76">
-        <v>65475290.353500001</v>
+        <v>65475290.350000001</v>
       </c>
       <c r="N76">
-        <v>67694647.592700005</v>
+        <v>67694647.590000004</v>
       </c>
       <c r="O76">
-        <v>59237651.351800002</v>
+        <v>59237651.350000001</v>
       </c>
       <c r="P76">
-        <v>56077561.474399999</v>
+        <v>56077561.469999999</v>
       </c>
       <c r="Q76">
         <v>54207405.409999996</v>
@@ -3867,22 +3869,22 @@
         <v>768.94</v>
       </c>
       <c r="L77">
-        <v>27880437.270300001</v>
+        <v>27880437.27</v>
       </c>
       <c r="M77">
-        <v>28389759.044</v>
+        <v>28389759.039999999</v>
       </c>
       <c r="N77">
-        <v>27913260.295400001</v>
+        <v>27913260.300000001</v>
       </c>
       <c r="O77">
-        <v>39816663.528999999</v>
+        <v>39816663.530000001</v>
       </c>
       <c r="P77">
-        <v>44101276.592500001</v>
+        <v>44101276.590000004</v>
       </c>
       <c r="Q77">
-        <v>43411662.291199997</v>
+        <v>43411662.289999999</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -3920,22 +3922,22 @@
         <v>621.66</v>
       </c>
       <c r="L78">
-        <v>21775405.563700002</v>
+        <v>21775405.559999999</v>
       </c>
       <c r="M78">
-        <v>23532222.5744</v>
+        <v>23532222.57</v>
       </c>
       <c r="N78">
-        <v>24850183.034699999</v>
+        <v>24850183.030000001</v>
       </c>
       <c r="O78">
-        <v>18841152.121199999</v>
+        <v>18841152.120000001</v>
       </c>
       <c r="P78">
-        <v>22892660.203000002</v>
+        <v>22892660.199999999</v>
       </c>
       <c r="Q78">
-        <v>21760739.432300001</v>
+        <v>21760739.43</v>
       </c>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
@@ -3973,22 +3975,22 @@
         <v>719.74</v>
       </c>
       <c r="L79">
-        <v>8652081.2982999999</v>
+        <v>8652081.2980000004</v>
       </c>
       <c r="M79">
-        <v>8068845.0382000003</v>
+        <v>8068845.0379999997</v>
       </c>
       <c r="N79">
-        <v>8480535.2914000005</v>
+        <v>8480535.2909999993</v>
       </c>
       <c r="O79">
-        <v>7567115.7922999999</v>
+        <v>7567115.7920000004</v>
       </c>
       <c r="P79">
-        <v>9299021.4272000007</v>
+        <v>9299021.4269999992</v>
       </c>
       <c r="Q79">
-        <v>8807513.5660999995</v>
+        <v>8807513.5659999996</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
@@ -4026,22 +4028,22 @@
         <v>1327.7</v>
       </c>
       <c r="L80">
-        <v>18300216.7073</v>
+        <v>18300216.710000001</v>
       </c>
       <c r="M80">
-        <v>18386757.304400001</v>
+        <v>18386757.300000001</v>
       </c>
       <c r="N80">
-        <v>16584466.957599999</v>
+        <v>16584466.960000001</v>
       </c>
       <c r="O80">
-        <v>10664352.801000001</v>
+        <v>10664352.800000001</v>
       </c>
       <c r="P80">
-        <v>12724569.7257</v>
+        <v>12724569.73</v>
       </c>
       <c r="Q80">
-        <v>13994405.776000001</v>
+        <v>13994405.779999999</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
@@ -4079,22 +4081,22 @@
         <v>727.4</v>
       </c>
       <c r="L81">
-        <v>8552283.8278999999</v>
+        <v>8552283.8279999997</v>
       </c>
       <c r="M81">
-        <v>7430405.0947000002</v>
+        <v>7430405.0949999997</v>
       </c>
       <c r="N81">
-        <v>8442646.2336999997</v>
+        <v>8442646.2339999992</v>
       </c>
       <c r="O81">
-        <v>10530094.7552</v>
+        <v>10530094.76</v>
       </c>
       <c r="P81">
-        <v>10328394.761499999</v>
+        <v>10328394.76</v>
       </c>
       <c r="Q81">
-        <v>12041933.178200001</v>
+        <v>12041933.18</v>
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
@@ -4135,19 +4137,19 @@
         <v>8419806.0460000001</v>
       </c>
       <c r="M82">
-        <v>7954686.9192000004</v>
+        <v>7954686.9189999998</v>
       </c>
       <c r="N82">
-        <v>8318226.5612000003</v>
+        <v>8318226.5609999998</v>
       </c>
       <c r="O82">
-        <v>8007517.5916999998</v>
+        <v>8007517.5920000002</v>
       </c>
       <c r="P82">
-        <v>7319791.0674000001</v>
+        <v>7319791.0669999998</v>
       </c>
       <c r="Q82">
-        <v>7367477.8015999999</v>
+        <v>7367477.8020000001</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
@@ -4185,22 +4187,22 @@
         <v>667.64</v>
       </c>
       <c r="L83">
-        <v>6594546.7669000002</v>
+        <v>6594546.767</v>
       </c>
       <c r="M83">
-        <v>6679574.3863000004</v>
+        <v>6679574.3859999999</v>
       </c>
       <c r="N83">
-        <v>6147241.6140999999</v>
+        <v>6147241.6140000001</v>
       </c>
       <c r="O83">
         <v>6238970.0020000003</v>
       </c>
       <c r="P83">
-        <v>6287508.4829000002</v>
+        <v>6287508.483</v>
       </c>
       <c r="Q83">
-        <v>7032912.1431999998</v>
+        <v>7032912.1430000002</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
@@ -4238,13 +4240,13 @@
         <v>777.81</v>
       </c>
       <c r="L84">
-        <v>1321073.9612</v>
+        <v>1321073.9609999999</v>
       </c>
       <c r="M84">
-        <v>1417953.1494</v>
+        <v>1417953.149</v>
       </c>
       <c r="N84">
-        <v>1424344.2490999999</v>
+        <v>1424344.2490000001</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -4291,22 +4293,22 @@
         <v>1314.56</v>
       </c>
       <c r="L85">
-        <v>1140127.9798999999</v>
+        <v>1140127.98</v>
       </c>
       <c r="M85">
         <v>1127351.3230000001</v>
       </c>
       <c r="N85">
-        <v>1111897.2497</v>
+        <v>1111897.25</v>
       </c>
       <c r="O85">
         <v>812868.51899999997</v>
       </c>
       <c r="P85">
-        <v>1002101.8837</v>
+        <v>1002101.884</v>
       </c>
       <c r="Q85">
-        <v>1019301.0618</v>
+        <v>1019301.062</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
@@ -4397,22 +4399,22 @@
         <v>727.4</v>
       </c>
       <c r="L87">
-        <v>5928286.9356000004</v>
+        <v>5928286.9359999998</v>
       </c>
       <c r="M87">
-        <v>5417515.3289000001</v>
+        <v>5417515.3289999999</v>
       </c>
       <c r="N87">
-        <v>5820192.7697000001</v>
+        <v>5820192.7699999996</v>
       </c>
       <c r="O87">
-        <v>6318313.4423000002</v>
+        <v>6318313.4419999998</v>
       </c>
       <c r="P87">
-        <v>7358851.5428999998</v>
+        <v>7358851.5429999996</v>
       </c>
       <c r="Q87">
-        <v>6698599.7855000002</v>
+        <v>6698599.7860000003</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
@@ -4453,19 +4455,19 @@
         <v>2465240.29</v>
       </c>
       <c r="M88">
-        <v>2312034.2787000001</v>
+        <v>2312034.2790000001</v>
       </c>
       <c r="N88">
-        <v>2478860.3385000001</v>
+        <v>2478860.3390000002</v>
       </c>
       <c r="O88">
-        <v>1261327.8343</v>
+        <v>1261327.834</v>
       </c>
       <c r="P88">
-        <v>1504831.4823</v>
+        <v>1504831.4820000001</v>
       </c>
       <c r="Q88">
-        <v>1670066.4952</v>
+        <v>1670066.4950000001</v>
       </c>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
@@ -4503,22 +4505,22 @@
         <v>455.72</v>
       </c>
       <c r="L89">
-        <v>1164487.3163999999</v>
+        <v>1164487.3160000001</v>
       </c>
       <c r="M89">
-        <v>1376477.9739000001</v>
+        <v>1376477.9739999999</v>
       </c>
       <c r="N89">
-        <v>1531498.6980999999</v>
+        <v>1531498.6980000001</v>
       </c>
       <c r="O89">
         <v>1398304.361</v>
       </c>
       <c r="P89">
-        <v>1633581.6309</v>
+        <v>1633581.6310000001</v>
       </c>
       <c r="Q89">
-        <v>2129396.5118</v>
+        <v>2129396.5120000001</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>